<commit_message>
update controltime period report
</commit_message>
<xml_diff>
--- a/resources/reports/employee/controltime_period_report.xlsx
+++ b/resources/reports/employee/controltime_period_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artem/PhpstormProjects/ControlPasec-Laravel/resources/reports/employee/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE00D3E1-FE63-0347-BD5B-F31824542028}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109D2646-9248-3243-AC7C-EA6B785B4EB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15340" xr2:uid="{1043D7AC-78CC-6746-A106-73C32A9C1A8A}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15140" xr2:uid="{1043D7AC-78CC-6746-A106-73C32A9C1A8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>{{ items.date }}</t>
-  </si>
-  <si>
     <t>Сотрудник</t>
   </si>
   <si>
@@ -42,13 +39,16 @@
     <t>Субъект</t>
   </si>
   <si>
-    <t>{{ items.employee }}</t>
-  </si>
-  <si>
-    <t>{{ items.hours }}</t>
-  </si>
-  <si>
-    <t>{{ items.subject }}</t>
+    <t>[employee]</t>
+  </si>
+  <si>
+    <t>[date]</t>
+  </si>
+  <si>
+    <t>[hours]</t>
+  </si>
+  <si>
+    <t>[subject]</t>
   </si>
 </sst>
 </file>
@@ -404,31 +404,36 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>

</xml_diff>